<commit_message>
keywords and locator helper
</commit_message>
<xml_diff>
--- a/resources/testcases.xlsx
+++ b/resources/testcases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t>BtnSubmit</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -571,7 +577,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +622,7 @@
         <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -685,6 +691,9 @@
       <c r="B2" t="s">
         <v>12</v>
       </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>

</xml_diff>